<commit_message>
Added log progress to user in windows
</commit_message>
<xml_diff>
--- a/src/Samples/MultilingualExtensionSampleUWP/Strings/en-US/Resources.resw.xlsx
+++ b/src/Samples/MultilingualExtensionSampleUWP/Strings/en-US/Resources.resw.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="12">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -26,13 +26,28 @@
     <t xml:space="preserve">Status</t>
   </si>
   <si>
+    <t xml:space="preserve">Cat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Need review</t>
+  </si>
+  <si>
     <t xml:space="preserve">Dog</t>
   </si>
   <si>
-    <t xml:space="preserve">Need review</t>
-  </si>
-  <si>
     <t xml:space="preserve">Hello</t>
+  </si>
+  <si>
+    <t xml:space="preserve">House</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Run if you like</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wood</t>
   </si>
 </sst>
 </file>
@@ -127,6 +142,81 @@
       </c>
       <c r="E3"/>
     </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>